<commit_message>
Fixed tests, padding, missing indices
</commit_message>
<xml_diff>
--- a/spec/fixtures/sample_import_assessments.xlsx
+++ b/spec/fixtures/sample_import_assessments.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10329"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dms3/Desktop/exercises/spec/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{6D1D0441-E734-2B4B-844C-2936FB3538F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{CB22215F-312B-8D46-B2B2-D66D793769EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17240" xr2:uid="{58324B81-82B1-E942-ADDD-32BBC418C366}"/>
+    <workbookView xWindow="1100" yWindow="780" windowWidth="28040" windowHeight="17240" xr2:uid="{58324B81-82B1-E942-ADDD-32BBC418C366}"/>
   </bookViews>
   <sheets>
     <sheet name="Evaluation World History Vol 1 " sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="29" uniqueCount="28">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="38" uniqueCount="37">
   <si>
     <t>Section</t>
   </si>
@@ -69,9 +69,6 @@
     <t>Post</t>
   </si>
   <si>
-    <t>Another question?</t>
-  </si>
-  <si>
     <t>Some question?</t>
   </si>
   <si>
@@ -109,6 +106,36 @@
   </si>
   <si>
     <t>6c30d0cc-e435-4081-be68-5ff2f558cbec</t>
+  </si>
+  <si>
+    <t>Nickname</t>
+  </si>
+  <si>
+    <t>Human TEKS</t>
+  </si>
+  <si>
+    <t>Machine TEKS</t>
+  </si>
+  <si>
+    <t>T1.1</t>
+  </si>
+  <si>
+    <t>T1.2</t>
+  </si>
+  <si>
+    <t>dacf53a6-2b09-49f1-9926-de4efe1049e0</t>
+  </si>
+  <si>
+    <t>c6623b8d-1eb7-41bf-875b-3456036000f9</t>
+  </si>
+  <si>
+    <t>Another question with \( R = a^i/se \) math?</t>
+  </si>
+  <si>
+    <t>Q1</t>
+  </si>
+  <si>
+    <t>Q2</t>
   </si>
 </sst>
 </file>
@@ -949,10 +976,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64FBECA4-7BDF-7B4A-92B0-936D12019FFC}">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -960,16 +987,18 @@
     <col min="1" max="1" width="7.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="35.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="23.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="35.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1000,31 +1029,40 @@
       <c r="J1" t="s">
         <v>6</v>
       </c>
+      <c r="K1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L1" t="s">
+        <v>28</v>
+      </c>
+      <c r="M1" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1.1000000000000001</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" t="s">
         <v>18</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>25</v>
-      </c>
-      <c r="G2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" t="s">
-        <v>26</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
@@ -1032,40 +1070,59 @@
       <c r="J2" t="s">
         <v>11</v>
       </c>
+      <c r="K2" t="s">
+        <v>35</v>
+      </c>
+      <c r="L2" t="s">
+        <v>30</v>
+      </c>
+      <c r="M2" t="s">
+        <v>32</v>
+      </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C3" t="s">
         <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="E3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" t="s">
         <v>20</v>
       </c>
-      <c r="F3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>21</v>
       </c>
-      <c r="H3" t="s">
-        <v>22</v>
-      </c>
       <c r="I3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3" t="s">
         <v>16</v>
       </c>
-      <c r="J3" t="s">
-        <v>17</v>
+      <c r="K3" t="s">
+        <v>36</v>
+      </c>
+      <c r="L3" t="s">
+        <v>31</v>
+      </c>
+      <c r="M3" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Test multipart, fix error when mixing normal and multipart
</commit_message>
<xml_diff>
--- a/spec/fixtures/sample_import_assessments.xlsx
+++ b/spec/fixtures/sample_import_assessments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dms3/Desktop/exercises/spec/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{CB22215F-312B-8D46-B2B2-D66D793769EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{2ED44C09-FB69-AE4C-8DDB-5829C4A7A687}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="780" windowWidth="28040" windowHeight="17240" xr2:uid="{58324B81-82B1-E942-ADDD-32BBC418C366}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="38" uniqueCount="37">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="51" uniqueCount="46">
   <si>
     <t>Section</t>
   </si>
@@ -136,6 +136,33 @@
   </si>
   <si>
     <t>Q2</t>
+  </si>
+  <si>
+    <t>Background</t>
+  </si>
+  <si>
+    <t>Oh look, multipart!</t>
+  </si>
+  <si>
+    <t>First part?</t>
+  </si>
+  <si>
+    <t>Second part?</t>
+  </si>
+  <si>
+    <t>Q3</t>
+  </si>
+  <si>
+    <t>T1.3</t>
+  </si>
+  <si>
+    <t>e6beb10a-f5cd-4b18-bf4a-e2f7174779bd</t>
+  </si>
+  <si>
+    <t>Multi Step Index</t>
+  </si>
+  <si>
+    <t>Block Index</t>
   </si>
 </sst>
 </file>
@@ -976,10 +1003,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64FBECA4-7BDF-7B4A-92B0-936D12019FFC}">
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:P5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -987,18 +1014,21 @@
     <col min="1" max="1" width="7.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="35.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="35.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="38.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="35.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1009,37 +1039,46 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>9</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>10</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>5</v>
       </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
         <v>6</v>
       </c>
-      <c r="K1" t="s">
+      <c r="N1" t="s">
         <v>27</v>
       </c>
-      <c r="L1" t="s">
+      <c r="O1" t="s">
         <v>28</v>
       </c>
-      <c r="M1" t="s">
+      <c r="P1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1.1000000000000001</v>
       </c>
@@ -1049,38 +1088,38 @@
       <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
+      <c r="G2" t="s">
         <v>14</v>
       </c>
-      <c r="E2" t="s">
+      <c r="H2" t="s">
         <v>17</v>
       </c>
-      <c r="F2" t="s">
+      <c r="I2" t="s">
         <v>24</v>
       </c>
-      <c r="G2" t="s">
+      <c r="J2" t="s">
         <v>18</v>
       </c>
-      <c r="H2" t="s">
+      <c r="K2" t="s">
         <v>25</v>
       </c>
-      <c r="I2" t="s">
+      <c r="L2" t="s">
         <v>8</v>
       </c>
-      <c r="J2" t="s">
+      <c r="M2" t="s">
         <v>11</v>
       </c>
-      <c r="K2" t="s">
+      <c r="N2" t="s">
         <v>35</v>
       </c>
-      <c r="L2" t="s">
+      <c r="O2" t="s">
         <v>30</v>
       </c>
-      <c r="M2" t="s">
+      <c r="P2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -1090,35 +1129,81 @@
       <c r="C3" t="s">
         <v>13</v>
       </c>
-      <c r="D3" t="s">
+      <c r="G3" t="s">
         <v>34</v>
       </c>
-      <c r="E3" t="s">
+      <c r="H3" t="s">
         <v>19</v>
       </c>
-      <c r="F3" t="s">
+      <c r="I3" t="s">
         <v>22</v>
       </c>
-      <c r="G3" t="s">
+      <c r="J3" t="s">
         <v>20</v>
       </c>
-      <c r="H3" t="s">
+      <c r="K3" t="s">
         <v>21</v>
       </c>
-      <c r="I3" t="s">
+      <c r="L3" t="s">
         <v>15</v>
       </c>
-      <c r="J3" t="s">
+      <c r="M3" t="s">
         <v>16</v>
       </c>
-      <c r="K3" t="s">
+      <c r="N3" t="s">
         <v>36</v>
       </c>
-      <c r="L3" t="s">
+      <c r="O3" t="s">
         <v>31</v>
       </c>
-      <c r="M3" t="s">
+      <c r="P3" t="s">
         <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
+        <v>38</v>
+      </c>
+      <c r="G4" t="s">
+        <v>40</v>
+      </c>
+      <c r="N4" t="s">
+        <v>41</v>
+      </c>
+      <c r="O4" t="s">
+        <v>42</v>
+      </c>
+      <c r="P4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G5" t="s">
+        <v>39</v>
+      </c>
+      <c r="N5" t="s">
+        <v>41</v>
+      </c>
+      <c r="O5" t="s">
+        <v>42</v>
+      </c>
+      <c r="P5" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added test for ancillary tag
</commit_message>
<xml_diff>
--- a/spec/fixtures/sample_import_assessments.xlsx
+++ b/spec/fixtures/sample_import_assessments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dms3/Desktop/exercises/spec/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{3BE28526-955E-204B-B258-FCB774821CE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{B6144A5A-C7DF-4B4A-9FFE-DFE19528653F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="780" windowWidth="28040" windowHeight="17240" xr2:uid="{58324B81-82B1-E942-ADDD-32BBC418C366}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="51" uniqueCount="46">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="53" uniqueCount="48">
   <si>
     <t>Section</t>
   </si>
@@ -163,6 +163,12 @@
   </si>
   <si>
     <t>&lt;p&gt;Oh look, multipart!&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Ancillary UUID</t>
+  </si>
+  <si>
+    <t>e9779614-2fca-43cb-ae53-4af6d20e00ea</t>
   </si>
 </sst>
 </file>
@@ -1003,10 +1009,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64FBECA4-7BDF-7B4A-92B0-936D12019FFC}">
-  <dimension ref="A1:P5"/>
+  <dimension ref="A1:Q5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1014,21 +1020,22 @@
     <col min="1" max="1" width="7.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="35.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="38.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="35.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="38.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="35.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1039,46 +1046,49 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" t="s">
         <v>43</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>44</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>37</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>2</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>3</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>4</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>5</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>6</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>27</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>28</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1.1000000000000001</v>
       </c>
@@ -1088,38 +1098,38 @@
       <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>14</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>17</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>24</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>18</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>25</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>8</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>11</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>35</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>30</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -1129,80 +1139,83 @@
       <c r="C3" t="s">
         <v>13</v>
       </c>
-      <c r="G3" t="s">
+      <c r="D3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H3" t="s">
         <v>34</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>19</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>22</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>20</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>21</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>15</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>16</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>36</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
         <v>31</v>
       </c>
-      <c r="P3" t="s">
+      <c r="Q3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="D4">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="E4">
         <v>0</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>1</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>45</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>39</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
         <v>40</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>41</v>
       </c>
-      <c r="P4" t="s">
+      <c r="Q4" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="D5">
-        <v>0</v>
-      </c>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="E5">
         <v>0</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5" t="s">
         <v>45</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>38</v>
       </c>
-      <c r="N5" t="s">
+      <c r="O5" t="s">
         <v>40</v>
       </c>
-      <c r="O5" t="s">
+      <c r="P5" t="s">
         <v>41</v>
       </c>
-      <c r="P5" t="s">
+      <c r="Q5" t="s">
         <v>42</v>
       </c>
     </row>

</xml_diff>